<commit_message>
removing *.epw and leaving * for weather
</commit_message>
<xml_diff>
--- a/projects/retail_ideal_calibration.xlsx
+++ b/projects/retail_ideal_calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2305,9 +2305,6 @@
     <t>../seeds/EmptySeedModel.osm</t>
   </si>
   <si>
-    <t>../weather/*.epw</t>
-  </si>
-  <si>
     <t>NGridAddMonthlyUtilityData</t>
   </si>
   <si>
@@ -2363,6 +2360,9 @@
   </si>
   <si>
     <t>Calibration Reports</t>
+  </si>
+  <si>
+    <t>../weather/*</t>
   </si>
 </sst>
 </file>
@@ -6387,8 +6387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6717,7 +6717,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>754</v>
+        <v>773</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6768,13 +6768,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
+        <v>767</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>766</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="B43" s="26" t="s">
-        <v>767</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6807,8 +6807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
@@ -7731,13 +7731,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E39" s="38" t="s">
         <v>69</v>
@@ -7750,16 +7750,16 @@
         <v>21</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F40" s="31" t="s">
         <v>622</v>
       </c>
       <c r="H40" s="31" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="I40" s="31"/>
     </row>
@@ -7768,16 +7768,16 @@
         <v>21</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F41" s="31" t="s">
         <v>622</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I41" s="31"/>
     </row>
@@ -7786,16 +7786,16 @@
         <v>21</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F42" s="31" t="s">
         <v>622</v>
       </c>
       <c r="H42" s="43" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I42" s="31"/>
     </row>
@@ -7804,16 +7804,16 @@
         <v>21</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>622</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="I43" s="31"/>
     </row>
@@ -7822,13 +7822,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E44" s="38" t="s">
         <v>234</v>

</xml_diff>